<commit_message>
Fix bugs: - Read formula
</commit_message>
<xml_diff>
--- a/RockyCommon/src_ut/SampleExcel.xlsx
+++ b/RockyCommon/src_ut/SampleExcel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15135" windowHeight="9300"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15135" windowHeight="9300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Data</t>
   </si>
@@ -49,13 +49,43 @@
   </si>
   <si>
     <t>New Data 5</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Double Formula</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>String Formular</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Date Formular</t>
+  </si>
+  <si>
+    <t>Date Func</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -81,14 +111,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -167,6 +205,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -201,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,24 +416,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -401,7 +441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -409,7 +449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -417,7 +457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -425,7 +465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -440,25 +480,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <f>6/10</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"A" &amp; "B"</f>
+        <v>AB</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2">
+        <v>40939</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <f ca="1">TODAY()</f>
+        <v>40921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3">
+        <f ca="1">B8+1</f>
+        <v>40922</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>